<commit_message>
made             #os.remove(os.path.join(settings.MEDIA_ROOT, name)) to work also
</commit_message>
<xml_diff>
--- a/media/format_tel_number/Customers1.xlsx
+++ b/media/format_tel_number/Customers1.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t> +46731264413</t>
+          <t>0731264413</t>
         </is>
       </c>
       <c r="G2" s="2" t="n"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t> 0046731212345</t>
+          <t>0731212345</t>
         </is>
       </c>
       <c r="G3" s="2" t="n"/>
@@ -520,7 +520,7 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>+4673123-4412</t>
+          <t>0731234412</t>
         </is>
       </c>
       <c r="G4" s="2" t="n"/>
@@ -551,7 +551,7 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>004673 123-3332</t>
+          <t>0731233332</t>
         </is>
       </c>
       <c r="G5" s="2" t="n"/>
@@ -582,7 +582,7 @@
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>076 111 12 34</t>
+          <t>0761111234</t>
         </is>
       </c>
       <c r="G6" s="2" t="n"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>75 113 1244</t>
+          <t>0751131244</t>
         </is>
       </c>
       <c r="G7" s="2" t="n"/>
@@ -644,7 +644,7 @@
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>08 444 555</t>
+          <t>08444555</t>
         </is>
       </c>
       <c r="G8" s="2" t="n"/>
@@ -675,7 +675,7 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t> 085556666</t>
+          <t>085556666</t>
         </is>
       </c>
       <c r="G9" s="2" t="n"/>
@@ -706,7 +706,7 @@
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t> 08-123-1234</t>
+          <t>081231234</t>
         </is>
       </c>
       <c r="G10" s="2" t="n"/>
@@ -737,7 +737,7 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>08555-6666</t>
+          <t>085556666</t>
         </is>
       </c>
       <c r="G11" s="2" t="n"/>

</xml_diff>